<commit_message>
New versions of submission forms
</commit_message>
<xml_diff>
--- a/docs/Alzymologist-submission-form.xlsx
+++ b/docs/Alzymologist-submission-form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darianechaeva/Desktop/Alzymologist /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA971EE3-70A6-8342-A53F-6FBF86A73EAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91214B5C-AF1F-EE4E-821B-723EF8AFDFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="1000" windowWidth="27840" windowHeight="15640" xr2:uid="{183F51DC-E21A-3B40-9A04-0B6DFD1DD036}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>Storage recommendations</t>
   </si>
   <si>
-    <t>Invoice should be sent to:</t>
-  </si>
-  <si>
     <t>Analytical report should be sent by</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Sample Submission Form</t>
   </si>
   <si>
-    <t>Number of submission form</t>
-  </si>
-  <si>
     <t>Real degree of fermentation, RDF</t>
   </si>
   <si>
@@ -172,6 +166,12 @@
   </si>
   <si>
     <t>Filled by the laboratory</t>
+  </si>
+  <si>
+    <t>Submission form number</t>
+  </si>
+  <si>
+    <t>Invoice should be sent to</t>
   </si>
 </sst>
 </file>
@@ -229,7 +229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -379,15 +379,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -399,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -420,6 +411,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -429,6 +441,36 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,6 +478,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -447,113 +504,35 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB4FB34-6B38-5149-BF8F-40F9C7FA72E3}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="99" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" zoomScalePageLayoutView="99" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScale="99" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" zoomScalePageLayoutView="99" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -915,34 +894,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="A1" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
@@ -957,12 +936,12 @@
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>22</v>
@@ -972,24 +951,24 @@
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
         <v>24</v>
@@ -997,16 +976,16 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1023,297 +1002,293 @@
         <v>26</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="46"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="A18" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="22"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="23" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="33"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="34"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="35"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="35"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="42"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="43"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
     </row>
     <row r="26" spans="1:7" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7" ht="8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" ht="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="E13:G18"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E13:G13"/>
     <mergeCell ref="A26:G31"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E19:G19"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
@@ -1323,21 +1298,25 @@
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E20:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.85578002244668905" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter>
+  <headerFooter alignWithMargins="0">
     <oddHeader xml:space="preserve">&amp;L&amp;"Calibri,обычный"&amp;K000000&amp;G&amp;C
 Alzymologist Oy
 &amp;R&amp;"PT Sans,обычный"&amp;K000000

</xml_diff>